<commit_message>
relecture et correction données métabo et analyses de survie
</commit_message>
<xml_diff>
--- a/20240928_label_metabo.xlsx
+++ b/20240928_label_metabo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/EXTENSION_MACMI/Analyses R/rstudio_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFDEE01-3FA8-A34D-8868-FAB3B735D405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595E2DDF-2BB8-2044-9B75-90EE77CBA89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{CE77C6B0-659B-BA41-A7C9-B5C9522E86B8}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CE77C6B0-659B-BA41-A7C9-B5C9522E86B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>label_metabo</t>
   </si>
@@ -155,7 +155,31 @@
     <t>moyenne_cibles_tep_4_suv_peak</t>
   </si>
   <si>
-    <t>label_survie</t>
+    <t>label_survie_all</t>
+  </si>
+  <si>
+    <t>label_survie_selected</t>
+  </si>
+  <si>
+    <t>index_4_0</t>
+  </si>
+  <si>
+    <t>index_4_2</t>
+  </si>
+  <si>
+    <t>index_2_0</t>
+  </si>
+  <si>
+    <t>index_suv_4_0</t>
+  </si>
+  <si>
+    <t>index_suv_4_2</t>
+  </si>
+  <si>
+    <t>index_suv_2_0</t>
+  </si>
+  <si>
+    <t>label_survie_index</t>
   </si>
 </sst>
 </file>
@@ -527,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12D713F-9CAB-2740-B89A-547CB79E2393}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,10 +562,11 @@
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +579,14 @@
       <c r="D1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -563,13 +594,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -577,13 +614,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -591,46 +634,79 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -640,8 +716,11 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -651,8 +730,11 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -662,8 +744,11 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -671,7 +756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -679,7 +764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -687,17 +772,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>29</v>
       </c>
@@ -745,6 +830,36 @@
     <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>